<commit_message>
2020-12-18 (minor update; ver 1.3.0.1)
Bugs
 - In `prnGSPA`, handled the case of more than one missing group of contrasts
   when computing fold changes etc. of contrasts.
 - In data preprocessing, devided the default `prot_cover` from Mascot by 100 for consistency.

Volcano plots
 - In `normPSM`,
   - added argument `rptr_intrange` for reporter-ion intensitity cut-offs by percentiles.
 - In volcano plots of`prnVol` or `pepVol`,
   - exported resultsfor custom plots (see `?prnVol` for example);
   - replaced `show_labels` with `topn_labels` for a custom number of top entries whenlabeling.
 - In volcano plots of`gspaMap`,
   - renamed argument `topn` to `topn_gsets` for clarity.
</commit_message>
<xml_diff>
--- a/inst/extdata/mascot_keys.xlsx
+++ b/inst/extdata/mascot_keys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Results\R\proteoQ\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36680217-ED05-4614-96F5-0F5662FEA221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD68F473-0F54-4C71-8A6C-A2F9250D1E2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="285">
   <si>
     <t>Header</t>
   </si>
@@ -863,9 +863,6 @@
     <t>Mascot sum of MS2 fragment-ion intensity of a peptide match</t>
   </si>
   <si>
-    <t>Mascot count of matched fragment ions of a peptide match</t>
-  </si>
-  <si>
     <r>
       <t>The second highest probablity, `</t>
     </r>
@@ -1293,6 +1290,12 @@
       </rPr>
       <t>Pep2Prn(method_pep_prn = ...)`</t>
     </r>
+  </si>
+  <si>
+    <t>Mascot count of matched and unmatched fragment ions of a peptide query</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSFragger at UniProt fasta(s): fasta_name(s) being used for non-primary protein(s). </t>
   </si>
 </sst>
 </file>
@@ -1815,8 +1818,8 @@
   <dimension ref="A1:C90"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1956,7 +1959,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="6" customFormat="1">
@@ -1973,7 +1976,7 @@
         <v>180</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C15" s="9"/>
     </row>
@@ -2081,7 +2084,7 @@
         <v>125</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="25.5">
@@ -2092,7 +2095,7 @@
         <v>161</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2114,7 +2117,7 @@
         <v>166</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2301,7 +2304,7 @@
         <v>186</v>
       </c>
       <c r="B49" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C49" s="18"/>
     </row>
@@ -2386,12 +2389,12 @@
       </c>
       <c r="C58" s="9"/>
     </row>
-    <row r="59" spans="1:3" s="32" customFormat="1" ht="12.75">
+    <row r="59" spans="1:3" s="32" customFormat="1" ht="25.5">
       <c r="A59" s="18" t="s">
         <v>179</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>231</v>
+        <v>283</v>
       </c>
       <c r="C59" s="9"/>
     </row>
@@ -2400,10 +2403,10 @@
         <v>85</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="32" customFormat="1" ht="12.75">
@@ -2420,7 +2423,7 @@
         <v>190</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C62" s="2"/>
     </row>
@@ -2429,7 +2432,7 @@
         <v>191</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C63" s="2"/>
     </row>
@@ -2438,10 +2441,10 @@
         <v>192</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="32" customFormat="1" ht="25.5">
@@ -2449,7 +2452,7 @@
         <v>193</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>98</v>
@@ -2460,7 +2463,7 @@
         <v>194</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>98</v>
@@ -2483,7 +2486,7 @@
         <v>145</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="32" customFormat="1" ht="12.75">
@@ -2549,12 +2552,15 @@
         <v>157</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" ht="25.5">
       <c r="A76" s="18" t="s">
         <v>188</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2562,7 +2568,7 @@
         <v>189</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2629,7 +2635,7 @@
         <v>79</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="25.5">
@@ -2637,7 +2643,7 @@
         <v>80</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>126</v>
@@ -2648,7 +2654,7 @@
         <v>82</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="25.5">
@@ -2656,7 +2662,7 @@
         <v>81</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>127</v>
@@ -2667,7 +2673,7 @@
         <v>83</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>128</v>
@@ -2678,7 +2684,7 @@
         <v>84</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -2696,8 +2702,8 @@
   <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2759,7 +2765,7 @@
         <v>180</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2887,10 +2893,10 @@
         <v>163</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2898,7 +2904,7 @@
         <v>164</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>98</v>
@@ -2909,7 +2915,7 @@
         <v>165</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>98</v>
@@ -2994,7 +3000,7 @@
         <v>186</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -3002,10 +3008,10 @@
         <v>48</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -3013,7 +3019,7 @@
         <v>49</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C32" s="18" t="s">
         <v>131</v>
@@ -3024,10 +3030,10 @@
         <v>85</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -3046,7 +3052,7 @@
         <v>190</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="25.5">
@@ -3054,7 +3060,7 @@
         <v>191</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="39">
@@ -3062,7 +3068,7 @@
         <v>87</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C37" s="16" t="s">
         <v>158</v>
@@ -3073,7 +3079,7 @@
         <v>88</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C38" s="16" t="s">
         <v>98</v>
@@ -3139,7 +3145,7 @@
         <v>94</v>
       </c>
       <c r="B44" s="17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C44" s="16" t="s">
         <v>98</v>
@@ -3150,7 +3156,7 @@
         <v>95</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C45" s="16" t="s">
         <v>98</v>
@@ -3274,16 +3280,18 @@
         <v>188</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="C58" s="18"/>
+        <v>239</v>
+      </c>
+      <c r="C58" s="25" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="59" spans="1:3" s="14" customFormat="1">
       <c r="A59" s="18" t="s">
         <v>189</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C59" s="18"/>
     </row>
@@ -3359,7 +3367,7 @@
         <v>20</v>
       </c>
       <c r="B67" s="25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C67" s="18" t="s">
         <v>132</v>
@@ -3370,7 +3378,7 @@
         <v>21</v>
       </c>
       <c r="B68" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C68" s="18" t="s">
         <v>133</v>
@@ -3381,7 +3389,7 @@
         <v>136</v>
       </c>
       <c r="B69" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>134</v>
@@ -3392,7 +3400,7 @@
         <v>137</v>
       </c>
       <c r="B70" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C70" s="18" t="s">
         <v>135</v>
@@ -3403,7 +3411,7 @@
         <v>138</v>
       </c>
       <c r="B71" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="25.5">
@@ -3429,8 +3437,8 @@
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3492,7 +3500,7 @@
         <v>180</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C6" s="7"/>
     </row>
@@ -3588,21 +3596,21 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>98</v>
@@ -3610,10 +3618,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>98</v>
@@ -3777,10 +3785,10 @@
         <v>20</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -3788,7 +3796,7 @@
         <v>21</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C38" s="2"/>
     </row>
@@ -3797,7 +3805,7 @@
         <v>137</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C39" s="2"/>
     </row>
@@ -3806,10 +3814,10 @@
         <v>138</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="25.5">
@@ -3817,7 +3825,7 @@
         <v>139</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C41" s="2"/>
     </row>

</xml_diff>